<commit_message>
Begin of interface part 2
</commit_message>
<xml_diff>
--- a/station_in_config/CoordinateSystem.xlsx
+++ b/station_in_config/CoordinateSystem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="435" windowWidth="10650" windowHeight="4455"/>
+    <workbookView xWindow="480" yWindow="255" windowWidth="10650" windowHeight="4455"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,7 +466,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Red color for error objects
</commit_message>
<xml_diff>
--- a/station_in_config/CoordinateSystem.xlsx
+++ b/station_in_config/CoordinateSystem.xlsx
@@ -412,7 +412,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -466,7 +466,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>

</xml_diff>